<commit_message>
Autorizacao do Download automaticamente e gerando mais de NF  de forma automática
</commit_message>
<xml_diff>
--- a/NotasEmitir.xlsx
+++ b/NotasEmitir.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaol\Desktop\Regravação Selenium\ex_01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bulllasa-my.sharepoint.com/personal/gabriel_souza_bullla_com_br/Documents/ws-hashtag-programacao/aut_emissao_nf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{868A8B7D-9A8A-4424-8DE5-566BF8816C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{868A8B7D-9A8A-4424-8DE5-566BF8816C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{031A5243-AB08-42B6-8D72-D17E2136B67B}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{E0C0BE46-0341-4CB7-B30B-1E97A67446E1}"/>
+    <workbookView xWindow="-38520" yWindow="2175" windowWidth="38640" windowHeight="15990" xr2:uid="{E0C0BE46-0341-4CB7-B30B-1E97A67446E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -819,12 +819,13 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="14.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" customWidth="1"/>
+    <col min="8" max="8" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -862,7 +863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -900,7 +901,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -938,7 +939,7 @@
         <v>4380</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -976,7 +977,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1014,7 +1015,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1052,7 +1053,7 @@
         <v>4797</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1090,7 +1091,7 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1128,7 +1129,7 @@
         <v>3728</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1166,7 +1167,7 @@
         <v>2440</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1204,7 +1205,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1242,7 +1243,7 @@
         <v>3176</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1280,7 +1281,7 @@
         <v>2940</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -1318,7 +1319,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -1356,7 +1357,7 @@
         <v>1952</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>71</v>
       </c>
@@ -1394,7 +1395,7 @@
         <v>3165</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>1410</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -1470,7 +1471,7 @@
         <v>3112</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -1508,7 +1509,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>89</v>
       </c>
@@ -1546,7 +1547,7 @@
         <v>4360</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>94</v>
       </c>
@@ -1584,7 +1585,7 @@
         <v>4074</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>98</v>
       </c>
@@ -1622,7 +1623,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -1660,7 +1661,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>107</v>
       </c>
@@ -1698,7 +1699,7 @@
         <v>6832</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>112</v>
       </c>
@@ -1736,7 +1737,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -1774,7 +1775,7 @@
         <v>2820</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>120</v>
       </c>
@@ -1812,7 +1813,7 @@
         <v>8208</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>123</v>
       </c>
@@ -1850,7 +1851,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>126</v>
       </c>
@@ -1888,7 +1889,7 @@
         <v>3804</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>130</v>
       </c>
@@ -1926,7 +1927,7 @@
         <v>3948</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>133</v>
       </c>
@@ -1964,7 +1965,7 @@
         <v>6559</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>137</v>
       </c>

</xml_diff>